<commit_message>
New Update due to changes
</commit_message>
<xml_diff>
--- a/Files/E-R Tables.xlsx
+++ b/Files/E-R Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ceu365-my.sharepoint.com/personal/amalia_rialplaza_usp_ceu_es/Documents/2°/2º Semestre/Bases de Datos/Proyect/IDSw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1251" documentId="8_{61BEFE8B-BC2E-41F6-814C-72C3817A851C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6160CA6-47EC-4060-BA9F-CEDAA52826B6}"/>
+  <xr:revisionPtr revIDLastSave="1367" documentId="8_{61BEFE8B-BC2E-41F6-814C-72C3817A851C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1DF3A5A-5034-4B7D-8A3B-34F0F49C24FD}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3F75AC25-16E0-4DDB-BA34-A14B622AD78F}"/>
+    <workbookView minimized="1" xWindow="2784" yWindow="2784" windowWidth="3012" windowHeight="720" xr2:uid="{3F75AC25-16E0-4DDB-BA34-A14B622AD78F}"/>
   </bookViews>
   <sheets>
     <sheet name="IDSw" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="129">
   <si>
     <t>Disease</t>
   </si>
@@ -65,9 +65,6 @@
     <t>AIDS</t>
   </si>
   <si>
-    <t>Virus (1)</t>
-  </si>
-  <si>
     <t>Symptom</t>
   </si>
   <si>
@@ -180,9 +177,6 @@
   </si>
   <si>
     <t>Sore Throat</t>
-  </si>
-  <si>
-    <t>Bacteria(2)</t>
   </si>
   <si>
     <t>HIV</t>
@@ -305,27 +299,12 @@
     <t>% Infected</t>
   </si>
   <si>
-    <t>Virus/Bact</t>
-  </si>
-  <si>
-    <t>Virus(1)</t>
-  </si>
-  <si>
     <t>Epstein-Barr</t>
   </si>
   <si>
     <t>Mononucleosis</t>
   </si>
   <si>
-    <t>Mild/ Severe</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mild (1)</t>
-  </si>
-  <si>
-    <t>Severe (2)</t>
-  </si>
-  <si>
     <t>Amoxicillin</t>
   </si>
   <si>
@@ -335,45 +314,12 @@
     <t>Foreign KEY</t>
   </si>
   <si>
-    <t>ill/ healthy/ immune/ deceased</t>
-  </si>
-  <si>
     <t>% Healthy</t>
   </si>
   <si>
     <t>Miopericarditis</t>
   </si>
   <si>
-    <t>Rodrigo Fernández Sanchez</t>
-  </si>
-  <si>
-    <t>Amalia Rial Plaza</t>
-  </si>
-  <si>
-    <t>Paula Rial Plaza</t>
-  </si>
-  <si>
-    <t>Victoria Rial Plaza</t>
-  </si>
-  <si>
-    <t>Sara Rial Villanueva</t>
-  </si>
-  <si>
-    <t>Rodrigo Rial Horcajo</t>
-  </si>
-  <si>
-    <t>Aranzazu Plaza Diaz</t>
-  </si>
-  <si>
-    <t>ill</t>
-  </si>
-  <si>
-    <t>healthy</t>
-  </si>
-  <si>
-    <t>immune</t>
-  </si>
-  <si>
     <t>Immunity Countdown</t>
   </si>
   <si>
@@ -389,9 +335,6 @@
     <t>Rifapentine</t>
   </si>
   <si>
-    <t>Rubén Garcia Pardo</t>
-  </si>
-  <si>
     <t>Azithromycin</t>
   </si>
   <si>
@@ -435,6 +378,63 @@
   </si>
   <si>
     <t>Inserted by researcher</t>
+  </si>
+  <si>
+    <t>Amalia</t>
+  </si>
+  <si>
+    <t>Paula</t>
+  </si>
+  <si>
+    <t>Victoria</t>
+  </si>
+  <si>
+    <t>Sara</t>
+  </si>
+  <si>
+    <t>Rodrigo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aranzazu </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rodrigo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rubén </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rial Plaza</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rial Villanueva</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rial Horcajo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Plaza Diaz</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fernández Sanchez</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Garcia Pardo</t>
+  </si>
+  <si>
+    <t>1(Mild)/2 (Severe)</t>
+  </si>
+  <si>
+    <t>1 (ill)/ 2 (healthy)/  3 (immune)</t>
+  </si>
+  <si>
+    <t>4 (deceased)</t>
+  </si>
+  <si>
+    <t>1 (Virus) /2 (Bacteria)</t>
+  </si>
+  <si>
+    <t>Surname</t>
   </si>
 </sst>
 </file>
@@ -602,7 +602,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -728,6 +728,12 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1077,8 +1083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44B747F3-0A34-43A6-91D2-0C931A04E494}">
   <dimension ref="A1:O142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="O99" sqref="O99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1088,7 +1094,7 @@
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.5546875" customWidth="1"/>
     <col min="7" max="7" width="25.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="26" bestFit="1" customWidth="1"/>
@@ -1107,7 +1113,7 @@
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
       <c r="C1" s="41" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -1134,11 +1140,11 @@
       <c r="I2" s="7"/>
       <c r="K2" s="4"/>
       <c r="L2" s="40" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M2" s="7"/>
       <c r="O2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -1148,22 +1154,22 @@
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4" t="s">
-        <v>85</v>
+        <v>127</v>
       </c>
       <c r="I3" s="9"/>
       <c r="K3" s="4"/>
       <c r="L3" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M3" s="9"/>
       <c r="O3" s="2" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -1171,7 +1177,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>2</v>
@@ -1180,13 +1186,13 @@
         <v>3</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="H4" s="13" t="s">
         <v>4</v>
@@ -1196,13 +1202,13 @@
       </c>
       <c r="K4" s="15"/>
       <c r="L4" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="M4" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="M4" s="17" t="s">
-        <v>17</v>
-      </c>
       <c r="O4" s="3" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -1210,7 +1216,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" s="4">
         <v>1.3</v>
@@ -1227,11 +1233,11 @@
       <c r="G5" s="4">
         <v>10</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>9</v>
+      <c r="H5" s="4">
+        <v>1</v>
       </c>
       <c r="I5" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K5" s="4"/>
       <c r="L5" s="8">
@@ -1246,7 +1252,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C6" s="4">
         <v>2.5</v>
@@ -1263,11 +1269,11 @@
       <c r="G6" s="19">
         <v>14</v>
       </c>
-      <c r="H6" s="4" t="s">
-        <v>48</v>
+      <c r="H6" s="4">
+        <v>2</v>
       </c>
       <c r="I6" s="18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K6" s="4"/>
       <c r="L6" s="8">
@@ -1299,11 +1305,11 @@
       <c r="G7" s="19">
         <v>4380</v>
       </c>
-      <c r="H7" s="4" t="s">
-        <v>9</v>
+      <c r="H7" s="4">
+        <v>1</v>
       </c>
       <c r="I7" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K7" s="4"/>
       <c r="L7" s="8">
@@ -1318,7 +1324,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C8" s="4">
         <v>2.5</v>
@@ -1335,11 +1341,11 @@
       <c r="G8" s="19">
         <v>14</v>
       </c>
-      <c r="H8" s="4" t="s">
-        <v>9</v>
+      <c r="H8" s="4">
+        <v>1</v>
       </c>
       <c r="I8" s="18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K8" s="4"/>
       <c r="L8" s="8">
@@ -1354,7 +1360,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C9" s="4">
         <v>4</v>
@@ -1371,11 +1377,11 @@
       <c r="G9" s="19">
         <v>12</v>
       </c>
-      <c r="H9" s="4" t="s">
-        <v>48</v>
+      <c r="H9" s="4">
+        <v>2</v>
       </c>
       <c r="I9" s="18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K9" s="4"/>
       <c r="L9" s="8">
@@ -1390,7 +1396,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C10" s="4">
         <v>2</v>
@@ -1407,11 +1413,11 @@
       <c r="G10" s="19">
         <v>14</v>
       </c>
-      <c r="H10" s="4" t="s">
-        <v>48</v>
+      <c r="H10" s="4">
+        <v>3</v>
       </c>
       <c r="I10" s="18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K10" s="4"/>
       <c r="L10" s="8">
@@ -1426,7 +1432,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C11" s="4">
         <v>1</v>
@@ -1443,11 +1449,11 @@
       <c r="G11" s="19">
         <v>2</v>
       </c>
-      <c r="H11" s="4" t="s">
-        <v>9</v>
+      <c r="H11" s="4">
+        <v>1</v>
       </c>
       <c r="I11" s="18" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="K11" s="4"/>
       <c r="L11" s="8">
@@ -1462,10 +1468,10 @@
         <v>8</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D12" s="42">
         <v>0.15</v>
@@ -1479,11 +1485,11 @@
       <c r="G12" s="19">
         <v>18</v>
       </c>
-      <c r="H12" s="4" t="s">
-        <v>48</v>
+      <c r="H12" s="4">
+        <v>2</v>
       </c>
       <c r="I12" s="18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K12" s="4"/>
       <c r="L12" s="8">
@@ -1498,7 +1504,7 @@
         <v>9</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C13" s="4">
         <v>9</v>
@@ -1515,11 +1521,11 @@
       <c r="G13" s="19">
         <v>13</v>
       </c>
-      <c r="H13" s="4" t="s">
-        <v>9</v>
+      <c r="H13" s="4">
+        <v>1</v>
       </c>
       <c r="I13" s="18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K13" s="4"/>
       <c r="L13" s="8">
@@ -1534,7 +1540,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C14" s="4">
         <v>5</v>
@@ -1551,11 +1557,11 @@
       <c r="G14" s="19">
         <v>210</v>
       </c>
-      <c r="H14" s="4" t="s">
-        <v>48</v>
+      <c r="H14" s="4">
+        <v>2</v>
       </c>
       <c r="I14" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K14" s="4"/>
       <c r="L14" s="8">
@@ -1570,7 +1576,7 @@
         <v>11</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C15" s="4">
         <v>2.5</v>
@@ -1587,11 +1593,11 @@
       <c r="G15" s="19">
         <v>7</v>
       </c>
-      <c r="H15" s="4" t="s">
-        <v>9</v>
+      <c r="H15" s="4">
+        <v>1</v>
       </c>
       <c r="I15" s="18" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K15" s="4"/>
       <c r="L15" s="8">
@@ -1623,11 +1629,11 @@
       <c r="G16" s="4">
         <v>21</v>
       </c>
-      <c r="H16" s="4" t="s">
-        <v>9</v>
+      <c r="H16" s="4">
+        <v>1</v>
       </c>
       <c r="I16" s="18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K16" s="4"/>
       <c r="L16" s="8">
@@ -1642,7 +1648,7 @@
         <v>13</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C17" s="22">
         <v>3.5</v>
@@ -1659,11 +1665,11 @@
       <c r="G17" s="22">
         <v>21</v>
       </c>
-      <c r="H17" s="22" t="s">
-        <v>86</v>
+      <c r="H17" s="22">
+        <v>1</v>
       </c>
       <c r="I17" s="23" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="K17" s="4"/>
       <c r="L17" s="8">
@@ -1713,7 +1719,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
@@ -1738,7 +1744,7 @@
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="9" t="s">
-        <v>89</v>
+        <v>124</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
@@ -1757,17 +1763,17 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
@@ -1787,10 +1793,10 @@
         <v>1</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>90</v>
+        <v>46</v>
+      </c>
+      <c r="C23" s="9">
+        <v>1</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="8"/>
@@ -1798,7 +1804,7 @@
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="J23" s="9"/>
       <c r="K23" s="4"/>
@@ -1814,29 +1820,29 @@
         <v>2</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>90</v>
+        <v>53</v>
+      </c>
+      <c r="C24" s="9">
+        <v>1</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H24" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F24" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="G24" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="H24" s="11" t="s">
+      <c r="I24" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="I24" s="11" t="s">
-        <v>23</v>
-      </c>
       <c r="J24" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K24" s="4"/>
       <c r="L24" s="8">
@@ -1851,10 +1857,10 @@
         <v>3</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>90</v>
+        <v>54</v>
+      </c>
+      <c r="C25" s="9">
+        <v>1</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="8">
@@ -1888,10 +1894,10 @@
         <v>4</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>90</v>
+        <v>55</v>
+      </c>
+      <c r="C26" s="9">
+        <v>1</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="8">
@@ -1925,10 +1931,10 @@
         <v>5</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>90</v>
+        <v>68</v>
+      </c>
+      <c r="C27" s="9">
+        <v>1</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="8">
@@ -1962,10 +1968,10 @@
         <v>6</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>90</v>
+        <v>57</v>
+      </c>
+      <c r="C28" s="9">
+        <v>1</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="21">
@@ -1999,10 +2005,10 @@
         <v>7</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>90</v>
+        <v>67</v>
+      </c>
+      <c r="C29" s="9">
+        <v>1</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
@@ -2024,10 +2030,10 @@
         <v>8</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>90</v>
+        <v>58</v>
+      </c>
+      <c r="C30" s="9">
+        <v>1</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
@@ -2049,10 +2055,10 @@
         <v>9</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>90</v>
+        <v>59</v>
+      </c>
+      <c r="C31" s="9">
+        <v>1</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -2074,10 +2080,10 @@
         <v>10</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>90</v>
+        <v>99</v>
+      </c>
+      <c r="C32" s="9">
+        <v>1</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
@@ -2099,10 +2105,10 @@
         <v>11</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>90</v>
+        <v>62</v>
+      </c>
+      <c r="C33" s="9">
+        <v>1</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
@@ -2124,10 +2130,10 @@
         <v>12</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>90</v>
+        <v>105</v>
+      </c>
+      <c r="C34" s="9">
+        <v>1</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
@@ -2149,16 +2155,18 @@
         <v>13</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>90</v>
+        <v>66</v>
+      </c>
+      <c r="C35" s="9">
+        <v>1</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F35" s="6"/>
+        <v>23</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>125</v>
+      </c>
       <c r="G35" s="6"/>
       <c r="H35" s="6"/>
       <c r="I35" s="7"/>
@@ -2176,18 +2184,18 @@
         <v>14</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>90</v>
+        <v>107</v>
+      </c>
+      <c r="C36" s="9">
+        <v>1</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="8"/>
       <c r="F36" s="4" t="s">
-        <v>95</v>
+        <v>126</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="H36" s="4"/>
       <c r="I36" s="9"/>
@@ -2205,26 +2213,26 @@
         <v>15</v>
       </c>
       <c r="B37" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="C37" s="24" t="s">
-        <v>90</v>
+        <v>63</v>
+      </c>
+      <c r="C37" s="24">
+        <v>1</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="10" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="F37" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G37" s="11" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="H37" s="11" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="I37" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
@@ -2240,17 +2248,17 @@
         <v>16</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>91</v>
+        <v>46</v>
+      </c>
+      <c r="C38" s="9">
+        <v>2</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="8">
         <v>1</v>
       </c>
-      <c r="F38" s="4" t="s">
-        <v>105</v>
+      <c r="F38" s="4">
+        <v>1</v>
       </c>
       <c r="G38" s="4">
         <v>20.5</v>
@@ -2275,17 +2283,17 @@
         <v>17</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>91</v>
+        <v>53</v>
+      </c>
+      <c r="C39" s="9">
+        <v>2</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="8">
         <v>2</v>
       </c>
-      <c r="F39" s="4" t="s">
-        <v>106</v>
+      <c r="F39" s="4">
+        <v>2</v>
       </c>
       <c r="G39" s="4">
         <v>0</v>
@@ -2310,17 +2318,17 @@
         <v>18</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>91</v>
+        <v>54</v>
+      </c>
+      <c r="C40" s="9">
+        <v>2</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="8">
         <v>3</v>
       </c>
-      <c r="F40" s="4" t="s">
-        <v>107</v>
+      <c r="F40" s="4">
+        <v>3</v>
       </c>
       <c r="G40" s="4">
         <v>0</v>
@@ -2345,17 +2353,17 @@
         <v>19</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>91</v>
+        <v>55</v>
+      </c>
+      <c r="C41" s="9">
+        <v>2</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="8">
         <v>4</v>
       </c>
-      <c r="F41" s="4" t="s">
-        <v>106</v>
+      <c r="F41" s="4">
+        <v>2</v>
       </c>
       <c r="G41" s="4">
         <v>0</v>
@@ -2380,17 +2388,17 @@
         <v>20</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>91</v>
+        <v>68</v>
+      </c>
+      <c r="C42" s="9">
+        <v>2</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="8">
         <v>5</v>
       </c>
-      <c r="F42" s="4" t="s">
-        <v>107</v>
+      <c r="F42" s="4">
+        <v>3</v>
       </c>
       <c r="G42" s="4">
         <v>0</v>
@@ -2415,17 +2423,17 @@
         <v>21</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>91</v>
+        <v>57</v>
+      </c>
+      <c r="C43" s="9">
+        <v>2</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="8">
         <v>6</v>
       </c>
-      <c r="F43" s="4" t="s">
-        <v>105</v>
+      <c r="F43" s="4">
+        <v>1</v>
       </c>
       <c r="G43" s="4">
         <v>20.5</v>
@@ -2450,17 +2458,17 @@
         <v>22</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>91</v>
+        <v>67</v>
+      </c>
+      <c r="C44" s="9">
+        <v>2</v>
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="8">
         <v>7</v>
       </c>
-      <c r="F44" s="4" t="s">
-        <v>105</v>
+      <c r="F44" s="4">
+        <v>1</v>
       </c>
       <c r="G44" s="4">
         <v>20.5</v>
@@ -2485,17 +2493,17 @@
         <v>23</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>91</v>
+        <v>58</v>
+      </c>
+      <c r="C45" s="9">
+        <v>2</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="8">
         <v>8</v>
       </c>
-      <c r="F45" s="4" t="s">
-        <v>105</v>
+      <c r="F45" s="4">
+        <v>1</v>
       </c>
       <c r="G45" s="4">
         <v>20.5</v>
@@ -2520,17 +2528,17 @@
         <v>24</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>91</v>
+        <v>59</v>
+      </c>
+      <c r="C46" s="9">
+        <v>2</v>
       </c>
       <c r="D46" s="4"/>
       <c r="E46" s="21">
         <v>9</v>
       </c>
-      <c r="F46" s="22" t="s">
-        <v>106</v>
+      <c r="F46" s="22">
+        <v>2</v>
       </c>
       <c r="G46" s="22">
         <v>0</v>
@@ -2555,17 +2563,17 @@
         <v>25</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>91</v>
+        <v>99</v>
+      </c>
+      <c r="C47" s="9">
+        <v>2</v>
       </c>
       <c r="D47" s="4"/>
       <c r="E47" s="32">
         <v>10</v>
       </c>
-      <c r="F47" s="6" t="s">
-        <v>105</v>
+      <c r="F47" s="6">
+        <v>1</v>
       </c>
       <c r="G47" s="6">
         <v>29</v>
@@ -2590,17 +2598,17 @@
         <v>26</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>91</v>
+        <v>62</v>
+      </c>
+      <c r="C48" s="9">
+        <v>2</v>
       </c>
       <c r="D48" s="4"/>
       <c r="E48" s="8">
         <v>11</v>
       </c>
-      <c r="F48" s="4" t="s">
-        <v>106</v>
+      <c r="F48" s="4">
+        <v>2</v>
       </c>
       <c r="G48" s="4">
         <v>0</v>
@@ -2625,17 +2633,17 @@
         <v>27</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>91</v>
+        <v>106</v>
+      </c>
+      <c r="C49" s="9">
+        <v>2</v>
       </c>
       <c r="D49" s="4"/>
       <c r="E49" s="8">
         <v>12</v>
       </c>
-      <c r="F49" s="4" t="s">
-        <v>107</v>
+      <c r="F49" s="4">
+        <v>3</v>
       </c>
       <c r="G49" s="4">
         <v>0</v>
@@ -2660,17 +2668,17 @@
         <v>28</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>91</v>
+        <v>66</v>
+      </c>
+      <c r="C50" s="9">
+        <v>2</v>
       </c>
       <c r="D50" s="4"/>
       <c r="E50" s="8">
         <v>13</v>
       </c>
-      <c r="F50" s="4" t="s">
-        <v>106</v>
+      <c r="F50" s="4">
+        <v>2</v>
       </c>
       <c r="G50" s="4">
         <v>0</v>
@@ -2695,17 +2703,17 @@
         <v>29</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="C51" s="9" t="s">
-        <v>91</v>
+        <v>107</v>
+      </c>
+      <c r="C51" s="9">
+        <v>2</v>
       </c>
       <c r="D51" s="4"/>
       <c r="E51" s="8">
         <v>14</v>
       </c>
-      <c r="F51" s="4" t="s">
-        <v>107</v>
+      <c r="F51" s="4">
+        <v>3</v>
       </c>
       <c r="G51" s="4">
         <v>0</v>
@@ -2730,17 +2738,17 @@
         <v>30</v>
       </c>
       <c r="B52" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="C52" s="24" t="s">
-        <v>91</v>
+        <v>63</v>
+      </c>
+      <c r="C52" s="24">
+        <v>2</v>
       </c>
       <c r="D52" s="4"/>
       <c r="E52" s="8">
         <v>15</v>
       </c>
-      <c r="F52" s="4" t="s">
-        <v>105</v>
+      <c r="F52" s="4">
+        <v>1</v>
       </c>
       <c r="G52" s="4">
         <v>29</v>
@@ -2768,8 +2776,8 @@
       <c r="E53" s="21">
         <v>16</v>
       </c>
-      <c r="F53" s="22" t="s">
-        <v>105</v>
+      <c r="F53" s="22">
+        <v>1</v>
       </c>
       <c r="G53" s="22">
         <v>29</v>
@@ -2797,8 +2805,8 @@
       <c r="E54" s="8">
         <v>17</v>
       </c>
-      <c r="F54" s="4" t="s">
-        <v>105</v>
+      <c r="F54" s="4">
+        <v>1</v>
       </c>
       <c r="G54" s="4">
         <v>22</v>
@@ -2826,8 +2834,8 @@
       <c r="E55" s="8">
         <v>18</v>
       </c>
-      <c r="F55" s="4" t="s">
-        <v>105</v>
+      <c r="F55" s="4">
+        <v>1</v>
       </c>
       <c r="G55" s="4">
         <v>22</v>
@@ -2855,8 +2863,8 @@
       <c r="E56" s="8">
         <v>19</v>
       </c>
-      <c r="F56" s="4" t="s">
-        <v>106</v>
+      <c r="F56" s="4">
+        <v>2</v>
       </c>
       <c r="G56" s="4">
         <v>0</v>
@@ -2878,7 +2886,7 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B57" s="6"/>
       <c r="C57" s="7"/>
@@ -2886,8 +2894,8 @@
       <c r="E57" s="8">
         <v>20</v>
       </c>
-      <c r="F57" s="4" t="s">
-        <v>105</v>
+      <c r="F57" s="4">
+        <v>1</v>
       </c>
       <c r="G57" s="4">
         <v>22</v>
@@ -2915,8 +2923,8 @@
       <c r="E58" s="8">
         <v>21</v>
       </c>
-      <c r="F58" s="4" t="s">
-        <v>106</v>
+      <c r="F58" s="4">
+        <v>2</v>
       </c>
       <c r="G58" s="4">
         <v>0</v>
@@ -2938,20 +2946,20 @@
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B59" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C59" s="17" t="s">
         <v>27</v>
-      </c>
-      <c r="C59" s="17" t="s">
-        <v>28</v>
       </c>
       <c r="D59" s="4"/>
       <c r="E59" s="21">
         <v>22</v>
       </c>
-      <c r="F59" s="22" t="s">
-        <v>107</v>
+      <c r="F59" s="22">
+        <v>3</v>
       </c>
       <c r="G59" s="22">
         <v>0</v>
@@ -2976,7 +2984,7 @@
         <v>1</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C60" s="9">
         <v>3</v>
@@ -2985,8 +2993,8 @@
       <c r="E60" s="8">
         <v>23</v>
       </c>
-      <c r="F60" s="4" t="s">
-        <v>106</v>
+      <c r="F60" s="4">
+        <v>2</v>
       </c>
       <c r="G60" s="4">
         <v>0</v>
@@ -3011,7 +3019,7 @@
         <v>2</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C61" s="9">
         <v>3</v>
@@ -3020,8 +3028,8 @@
       <c r="E61" s="8">
         <v>24</v>
       </c>
-      <c r="F61" s="4" t="s">
-        <v>105</v>
+      <c r="F61" s="4">
+        <v>1</v>
       </c>
       <c r="G61" s="4">
         <v>98</v>
@@ -3046,7 +3054,7 @@
         <v>3</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="C62" s="9">
         <v>1</v>
@@ -3055,8 +3063,8 @@
       <c r="E62" s="8">
         <v>25</v>
       </c>
-      <c r="F62" s="4" t="s">
-        <v>106</v>
+      <c r="F62" s="4">
+        <v>2</v>
       </c>
       <c r="G62" s="4">
         <v>0</v>
@@ -3081,7 +3089,7 @@
         <v>4</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C63" s="9">
         <v>7</v>
@@ -3090,8 +3098,8 @@
       <c r="E63" s="8">
         <v>26</v>
       </c>
-      <c r="F63" s="4" t="s">
-        <v>107</v>
+      <c r="F63" s="4">
+        <v>3</v>
       </c>
       <c r="G63" s="4">
         <v>0</v>
@@ -3116,7 +3124,7 @@
         <v>5</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C64" s="9">
         <v>3</v>
@@ -3125,8 +3133,8 @@
       <c r="E64" s="8">
         <v>27</v>
       </c>
-      <c r="F64" s="4" t="s">
-        <v>106</v>
+      <c r="F64" s="4">
+        <v>2</v>
       </c>
       <c r="G64" s="4">
         <v>0</v>
@@ -3151,7 +3159,7 @@
         <v>6</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="C65" s="9">
         <v>4</v>
@@ -3160,14 +3168,14 @@
       <c r="E65" s="21">
         <v>28</v>
       </c>
-      <c r="F65" s="22" t="s">
-        <v>107</v>
+      <c r="F65" s="22">
+        <v>3</v>
       </c>
       <c r="G65" s="22">
         <v>0</v>
       </c>
       <c r="H65" s="22">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="I65" s="24">
         <v>13</v>
@@ -3186,7 +3194,7 @@
         <v>7</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="C66" s="9">
         <v>1</v>
@@ -3211,7 +3219,7 @@
         <v>8</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="C67" s="9">
         <v>10</v>
@@ -3236,7 +3244,7 @@
         <v>9</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="C68" s="9">
         <v>8</v>
@@ -3261,7 +3269,7 @@
         <v>10</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="C69" s="9">
         <v>6</v>
@@ -3286,7 +3294,7 @@
         <v>11</v>
       </c>
       <c r="B70" s="22" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="C70" s="24">
         <v>2</v>
@@ -3314,7 +3322,7 @@
       <c r="E71" s="4"/>
       <c r="F71" s="4"/>
       <c r="G71" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H71" s="7"/>
       <c r="I71" s="4"/>
@@ -3348,7 +3356,7 @@
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B73" s="6"/>
       <c r="C73" s="6"/>
@@ -3356,10 +3364,10 @@
       <c r="E73" s="7"/>
       <c r="F73" s="4"/>
       <c r="G73" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H73" s="17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I73" s="4"/>
       <c r="J73" s="4"/>
@@ -3396,19 +3404,19 @@
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B75" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C75" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C75" s="11" t="s">
+      <c r="D75" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="E75" s="17" t="s">
         <v>34</v>
-      </c>
-      <c r="D75" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="E75" s="17" t="s">
-        <v>35</v>
       </c>
       <c r="F75" s="4"/>
       <c r="G75" s="8">
@@ -3432,7 +3440,7 @@
         <v>1</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C76" s="34">
         <v>36699</v>
@@ -3465,7 +3473,7 @@
         <v>2</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C77" s="34">
         <v>45177</v>
@@ -3498,7 +3506,7 @@
         <v>3</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C78" s="34">
         <v>45374</v>
@@ -3531,7 +3539,7 @@
         <v>4</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C79" s="34">
         <v>41130</v>
@@ -3564,7 +3572,7 @@
         <v>5</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C80" s="34">
         <v>45323</v>
@@ -3597,7 +3605,7 @@
         <v>6</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C81" s="34">
         <v>43957</v>
@@ -3630,7 +3638,7 @@
         <v>7</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C82" s="34">
         <v>44488</v>
@@ -3663,7 +3671,7 @@
         <v>8</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C83" s="34">
         <v>39219</v>
@@ -3696,7 +3704,7 @@
         <v>9</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C84" s="34">
         <v>45364</v>
@@ -3729,7 +3737,7 @@
         <v>10</v>
       </c>
       <c r="B85" s="22" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C85" s="35">
         <v>41604</v>
@@ -3812,16 +3820,16 @@
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B89" s="36"/>
       <c r="C89" s="15"/>
       <c r="D89" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E89" s="37"/>
-      <c r="F89" s="36"/>
-      <c r="G89" s="4"/>
+      <c r="F89" s="37"/>
+      <c r="G89" s="7"/>
       <c r="H89" s="4"/>
       <c r="I89" s="4"/>
       <c r="J89" s="4"/>
@@ -3838,9 +3846,9 @@
       <c r="B90" s="9"/>
       <c r="C90" s="4"/>
       <c r="D90" s="8"/>
-      <c r="E90" s="4"/>
-      <c r="F90" s="9"/>
-      <c r="G90" s="4"/>
+      <c r="E90" s="45"/>
+      <c r="F90" s="45"/>
+      <c r="G90" s="9"/>
       <c r="H90" s="4"/>
       <c r="I90" s="4"/>
       <c r="J90" s="4"/>
@@ -3854,22 +3862,24 @@
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A91" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B91" s="17" t="s">
         <v>38</v>
-      </c>
-      <c r="B91" s="17" t="s">
-        <v>39</v>
       </c>
       <c r="C91" s="15"/>
       <c r="D91" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E91" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="E91" s="11" t="s">
+      <c r="F91" s="46" t="s">
+        <v>128</v>
+      </c>
+      <c r="G91" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="F91" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="G91" s="4"/>
       <c r="H91" s="4"/>
       <c r="I91" s="4"/>
       <c r="J91" s="4"/>
@@ -3892,13 +3902,15 @@
       <c r="D92" s="8">
         <v>1</v>
       </c>
-      <c r="E92" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="F92" s="38">
+      <c r="E92" s="45" t="s">
+        <v>110</v>
+      </c>
+      <c r="F92" s="45" t="s">
+        <v>118</v>
+      </c>
+      <c r="G92" s="38">
         <v>38171</v>
       </c>
-      <c r="G92" s="4"/>
       <c r="H92" s="4"/>
       <c r="I92" s="4"/>
       <c r="J92" s="4"/>
@@ -3921,13 +3933,15 @@
       <c r="D93" s="8">
         <v>2</v>
       </c>
-      <c r="E93" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="F93" s="38">
+      <c r="E93" s="45" t="s">
+        <v>111</v>
+      </c>
+      <c r="F93" s="45" t="s">
+        <v>118</v>
+      </c>
+      <c r="G93" s="38">
         <v>37097</v>
       </c>
-      <c r="G93" s="4"/>
       <c r="H93" s="4"/>
       <c r="I93" s="4"/>
       <c r="J93" s="4"/>
@@ -3950,13 +3964,15 @@
       <c r="D94" s="8">
         <v>3</v>
       </c>
-      <c r="E94" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="F94" s="38">
+      <c r="E94" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="F94" s="45" t="s">
+        <v>118</v>
+      </c>
+      <c r="G94" s="38">
         <v>36516</v>
       </c>
-      <c r="G94" s="4"/>
       <c r="H94" s="4"/>
       <c r="I94" s="4"/>
       <c r="J94" s="4"/>
@@ -3979,13 +3995,15 @@
       <c r="D95" s="8">
         <v>4</v>
       </c>
-      <c r="E95" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="F95" s="38">
+      <c r="E95" s="45" t="s">
+        <v>113</v>
+      </c>
+      <c r="F95" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="G95" s="38">
         <v>33395</v>
       </c>
-      <c r="G95" s="4"/>
       <c r="H95" s="4"/>
       <c r="I95" s="4"/>
       <c r="J95" s="4"/>
@@ -4008,13 +4026,15 @@
       <c r="D96" s="8">
         <v>5</v>
       </c>
-      <c r="E96" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F96" s="38">
+      <c r="E96" s="45" t="s">
+        <v>114</v>
+      </c>
+      <c r="F96" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="G96" s="38">
         <v>22882</v>
       </c>
-      <c r="G96" s="4"/>
       <c r="H96" s="4"/>
       <c r="I96" s="4"/>
       <c r="J96" s="4"/>
@@ -4037,13 +4057,15 @@
       <c r="D97" s="8">
         <v>6</v>
       </c>
-      <c r="E97" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="F97" s="38">
+      <c r="E97" s="45" t="s">
+        <v>115</v>
+      </c>
+      <c r="F97" s="45" t="s">
+        <v>121</v>
+      </c>
+      <c r="G97" s="38">
         <v>26375</v>
       </c>
-      <c r="G97" s="4"/>
       <c r="H97" s="4"/>
       <c r="I97" s="4"/>
       <c r="J97" s="4"/>
@@ -4066,13 +4088,15 @@
       <c r="D98" s="8">
         <v>7</v>
       </c>
-      <c r="E98" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="F98" s="38">
+      <c r="E98" s="45" t="s">
+        <v>116</v>
+      </c>
+      <c r="F98" s="45" t="s">
+        <v>122</v>
+      </c>
+      <c r="G98" s="38">
         <v>38121</v>
       </c>
-      <c r="G98" s="4"/>
       <c r="H98" s="4"/>
       <c r="I98" s="4"/>
       <c r="J98" s="4"/>
@@ -4096,12 +4120,14 @@
         <v>8</v>
       </c>
       <c r="E99" s="22" t="s">
-        <v>113</v>
-      </c>
-      <c r="F99" s="39">
+        <v>117</v>
+      </c>
+      <c r="F99" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="G99" s="39">
         <v>37913</v>
       </c>
-      <c r="G99" s="4"/>
       <c r="H99" s="4"/>
       <c r="I99" s="4"/>
       <c r="J99" s="4"/>
@@ -4932,7 +4958,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="32" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="30" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Excel file of the E-R Tables
</commit_message>
<xml_diff>
--- a/Files/E-R Tables.xlsx
+++ b/Files/E-R Tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ceu365-my.sharepoint.com/personal/amalia_rialplaza_usp_ceu_es/Documents/2°/2º Semestre/Bases de Datos/Proyect/IDSw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1367" documentId="8_{61BEFE8B-BC2E-41F6-814C-72C3817A851C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1DF3A5A-5034-4B7D-8A3B-34F0F49C24FD}"/>
+  <xr:revisionPtr revIDLastSave="1433" documentId="8_{61BEFE8B-BC2E-41F6-814C-72C3817A851C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62A5B03A-9F28-4683-B0AC-D7029A745A5A}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2784" yWindow="2784" windowWidth="3012" windowHeight="720" xr2:uid="{3F75AC25-16E0-4DDB-BA34-A14B622AD78F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3F75AC25-16E0-4DDB-BA34-A14B622AD78F}"/>
   </bookViews>
   <sheets>
     <sheet name="IDSw" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="133">
   <si>
     <t>Disease</t>
   </si>
@@ -422,19 +422,31 @@
     <t xml:space="preserve"> Garcia Pardo</t>
   </si>
   <si>
-    <t>1(Mild)/2 (Severe)</t>
-  </si>
-  <si>
-    <t>1 (ill)/ 2 (healthy)/  3 (immune)</t>
-  </si>
-  <si>
-    <t>4 (deceased)</t>
-  </si>
-  <si>
-    <t>1 (Virus) /2 (Bacteria)</t>
-  </si>
-  <si>
     <t>Surname</t>
+  </si>
+  <si>
+    <t>Diagnosis has treatment</t>
+  </si>
+  <si>
+    <t>VIRUS</t>
+  </si>
+  <si>
+    <t>BACTERIA</t>
+  </si>
+  <si>
+    <t>MILD</t>
+  </si>
+  <si>
+    <t>SEVERE</t>
+  </si>
+  <si>
+    <t>ILL</t>
+  </si>
+  <si>
+    <t>HEALTHY</t>
+  </si>
+  <si>
+    <t>IMMUNE</t>
   </si>
 </sst>
 </file>
@@ -730,10 +742,10 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1081,10 +1093,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44B747F3-0A34-43A6-91D2-0C931A04E494}">
-  <dimension ref="A1:O142"/>
+  <dimension ref="A1:M142"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="O99" sqref="O99"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1109,7 +1121,7 @@
     <col min="19" max="19" width="15.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
       <c r="C1" s="41" t="s">
@@ -1126,7 +1138,7 @@
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1143,11 +1155,8 @@
         <v>14</v>
       </c>
       <c r="M2" s="7"/>
-      <c r="O2" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>6</v>
       </c>
@@ -1159,20 +1168,15 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
-      <c r="H3" s="4" t="s">
-        <v>127</v>
-      </c>
+      <c r="H3" s="4"/>
       <c r="I3" s="9"/>
       <c r="K3" s="4"/>
       <c r="L3" s="8" t="s">
         <v>17</v>
       </c>
       <c r="M3" s="9"/>
-      <c r="O3" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>1</v>
       </c>
@@ -1207,11 +1211,8 @@
       <c r="M4" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="O4" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>1</v>
       </c>
@@ -1233,8 +1234,8 @@
       <c r="G5" s="4">
         <v>10</v>
       </c>
-      <c r="H5" s="4">
-        <v>1</v>
+      <c r="H5" s="4" t="s">
+        <v>126</v>
       </c>
       <c r="I5" s="18" t="s">
         <v>45</v>
@@ -1247,7 +1248,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>2</v>
       </c>
@@ -1269,8 +1270,8 @@
       <c r="G6" s="19">
         <v>14</v>
       </c>
-      <c r="H6" s="4">
-        <v>2</v>
+      <c r="H6" s="4" t="s">
+        <v>127</v>
       </c>
       <c r="I6" s="18" t="s">
         <v>52</v>
@@ -1283,7 +1284,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>3</v>
       </c>
@@ -1305,8 +1306,8 @@
       <c r="G7" s="19">
         <v>4380</v>
       </c>
-      <c r="H7" s="4">
-        <v>1</v>
+      <c r="H7" s="4" t="s">
+        <v>126</v>
       </c>
       <c r="I7" s="18" t="s">
         <v>47</v>
@@ -1319,7 +1320,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>4</v>
       </c>
@@ -1341,8 +1342,8 @@
       <c r="G8" s="19">
         <v>14</v>
       </c>
-      <c r="H8" s="4">
-        <v>1</v>
+      <c r="H8" s="4" t="s">
+        <v>126</v>
       </c>
       <c r="I8" s="18" t="s">
         <v>64</v>
@@ -1355,7 +1356,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>5</v>
       </c>
@@ -1377,8 +1378,8 @@
       <c r="G9" s="19">
         <v>12</v>
       </c>
-      <c r="H9" s="4">
-        <v>2</v>
+      <c r="H9" s="4" t="s">
+        <v>127</v>
       </c>
       <c r="I9" s="18" t="s">
         <v>78</v>
@@ -1391,7 +1392,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <v>6</v>
       </c>
@@ -1413,8 +1414,8 @@
       <c r="G10" s="19">
         <v>14</v>
       </c>
-      <c r="H10" s="4">
-        <v>3</v>
+      <c r="H10" s="4" t="s">
+        <v>127</v>
       </c>
       <c r="I10" s="18" t="s">
         <v>73</v>
@@ -1427,7 +1428,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>7</v>
       </c>
@@ -1449,8 +1450,8 @@
       <c r="G11" s="19">
         <v>2</v>
       </c>
-      <c r="H11" s="4">
-        <v>1</v>
+      <c r="H11" s="4" t="s">
+        <v>126</v>
       </c>
       <c r="I11" s="18" t="s">
         <v>91</v>
@@ -1463,7 +1464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="8">
         <v>8</v>
       </c>
@@ -1485,8 +1486,8 @@
       <c r="G12" s="19">
         <v>18</v>
       </c>
-      <c r="H12" s="4">
-        <v>2</v>
+      <c r="H12" s="4" t="s">
+        <v>127</v>
       </c>
       <c r="I12" s="18" t="s">
         <v>77</v>
@@ -1499,7 +1500,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="8">
         <v>9</v>
       </c>
@@ -1521,8 +1522,8 @@
       <c r="G13" s="19">
         <v>13</v>
       </c>
-      <c r="H13" s="4">
-        <v>1</v>
+      <c r="H13" s="4" t="s">
+        <v>126</v>
       </c>
       <c r="I13" s="18" t="s">
         <v>76</v>
@@ -1535,7 +1536,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="8">
         <v>10</v>
       </c>
@@ -1557,8 +1558,8 @@
       <c r="G14" s="19">
         <v>210</v>
       </c>
-      <c r="H14" s="4">
-        <v>2</v>
+      <c r="H14" s="4" t="s">
+        <v>127</v>
       </c>
       <c r="I14" s="18" t="s">
         <v>71</v>
@@ -1571,7 +1572,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
         <v>11</v>
       </c>
@@ -1593,8 +1594,8 @@
       <c r="G15" s="19">
         <v>7</v>
       </c>
-      <c r="H15" s="4">
-        <v>1</v>
+      <c r="H15" s="4" t="s">
+        <v>126</v>
       </c>
       <c r="I15" s="18" t="s">
         <v>70</v>
@@ -1607,7 +1608,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
         <v>12</v>
       </c>
@@ -1629,8 +1630,8 @@
       <c r="G16" s="4">
         <v>21</v>
       </c>
-      <c r="H16" s="4">
-        <v>1</v>
+      <c r="H16" s="4" t="s">
+        <v>126</v>
       </c>
       <c r="I16" s="18" t="s">
         <v>75</v>
@@ -1665,8 +1666,8 @@
       <c r="G17" s="22">
         <v>21</v>
       </c>
-      <c r="H17" s="22">
-        <v>1</v>
+      <c r="H17" s="22" t="s">
+        <v>126</v>
       </c>
       <c r="I17" s="23" t="s">
         <v>83</v>
@@ -1743,9 +1744,7 @@
         <v>6</v>
       </c>
       <c r="B21" s="4"/>
-      <c r="C21" s="9" t="s">
-        <v>124</v>
-      </c>
+      <c r="C21" s="9"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
@@ -1795,8 +1794,8 @@
       <c r="B23" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="9">
-        <v>1</v>
+      <c r="C23" s="9" t="s">
+        <v>128</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="8"/>
@@ -1822,8 +1821,8 @@
       <c r="B24" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="9">
-        <v>1</v>
+      <c r="C24" s="9" t="s">
+        <v>128</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="26" t="s">
@@ -1859,8 +1858,8 @@
       <c r="B25" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C25" s="9">
-        <v>1</v>
+      <c r="C25" s="9" t="s">
+        <v>128</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="8">
@@ -1896,8 +1895,8 @@
       <c r="B26" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="9">
-        <v>1</v>
+      <c r="C26" s="9" t="s">
+        <v>128</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="8">
@@ -1933,8 +1932,8 @@
       <c r="B27" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C27" s="9">
-        <v>1</v>
+      <c r="C27" s="9" t="s">
+        <v>128</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="8">
@@ -1970,8 +1969,8 @@
       <c r="B28" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C28" s="9">
-        <v>1</v>
+      <c r="C28" s="9" t="s">
+        <v>128</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="21">
@@ -2007,8 +2006,8 @@
       <c r="B29" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C29" s="9">
-        <v>1</v>
+      <c r="C29" s="9" t="s">
+        <v>128</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
@@ -2032,8 +2031,8 @@
       <c r="B30" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="9">
-        <v>1</v>
+      <c r="C30" s="9" t="s">
+        <v>128</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
@@ -2057,8 +2056,8 @@
       <c r="B31" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="9">
-        <v>1</v>
+      <c r="C31" s="9" t="s">
+        <v>128</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -2082,8 +2081,8 @@
       <c r="B32" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C32" s="9">
-        <v>1</v>
+      <c r="C32" s="9" t="s">
+        <v>128</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
@@ -2107,8 +2106,8 @@
       <c r="B33" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C33" s="9">
-        <v>1</v>
+      <c r="C33" s="9" t="s">
+        <v>128</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
@@ -2132,8 +2131,8 @@
       <c r="B34" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C34" s="9">
-        <v>1</v>
+      <c r="C34" s="9" t="s">
+        <v>128</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
@@ -2157,16 +2156,14 @@
       <c r="B35" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C35" s="9">
-        <v>1</v>
+      <c r="C35" s="9" t="s">
+        <v>128</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F35" s="6" t="s">
-        <v>125</v>
-      </c>
+      <c r="F35" s="6"/>
       <c r="G35" s="6"/>
       <c r="H35" s="6"/>
       <c r="I35" s="7"/>
@@ -2186,14 +2183,12 @@
       <c r="B36" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="C36" s="9">
-        <v>1</v>
+      <c r="C36" s="9" t="s">
+        <v>128</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="8"/>
-      <c r="F36" s="4" t="s">
-        <v>126</v>
-      </c>
+      <c r="F36" s="4"/>
       <c r="G36" s="4" t="s">
         <v>101</v>
       </c>
@@ -2215,8 +2210,8 @@
       <c r="B37" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="C37" s="24">
-        <v>1</v>
+      <c r="C37" s="24" t="s">
+        <v>128</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="10" t="s">
@@ -2250,15 +2245,15 @@
       <c r="B38" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C38" s="9">
-        <v>2</v>
+      <c r="C38" s="9" t="s">
+        <v>129</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="8">
         <v>1</v>
       </c>
-      <c r="F38" s="4">
-        <v>1</v>
+      <c r="F38" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="G38" s="4">
         <v>20.5</v>
@@ -2285,15 +2280,15 @@
       <c r="B39" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C39" s="9">
-        <v>2</v>
+      <c r="C39" s="9" t="s">
+        <v>129</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="8">
         <v>2</v>
       </c>
-      <c r="F39" s="4">
-        <v>2</v>
+      <c r="F39" s="4" t="s">
+        <v>131</v>
       </c>
       <c r="G39" s="4">
         <v>0</v>
@@ -2320,15 +2315,15 @@
       <c r="B40" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C40" s="9">
-        <v>2</v>
+      <c r="C40" s="9" t="s">
+        <v>129</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="8">
         <v>3</v>
       </c>
-      <c r="F40" s="4">
-        <v>3</v>
+      <c r="F40" s="4" t="s">
+        <v>132</v>
       </c>
       <c r="G40" s="4">
         <v>0</v>
@@ -2355,15 +2350,15 @@
       <c r="B41" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C41" s="9">
-        <v>2</v>
+      <c r="C41" s="9" t="s">
+        <v>129</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="8">
         <v>4</v>
       </c>
-      <c r="F41" s="4">
-        <v>2</v>
+      <c r="F41" s="4" t="s">
+        <v>131</v>
       </c>
       <c r="G41" s="4">
         <v>0</v>
@@ -2390,15 +2385,15 @@
       <c r="B42" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C42" s="9">
-        <v>2</v>
+      <c r="C42" s="9" t="s">
+        <v>129</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="8">
         <v>5</v>
       </c>
-      <c r="F42" s="4">
-        <v>3</v>
+      <c r="F42" s="4" t="s">
+        <v>132</v>
       </c>
       <c r="G42" s="4">
         <v>0</v>
@@ -2425,15 +2420,15 @@
       <c r="B43" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C43" s="9">
-        <v>2</v>
+      <c r="C43" s="9" t="s">
+        <v>129</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="8">
         <v>6</v>
       </c>
-      <c r="F43" s="4">
-        <v>1</v>
+      <c r="F43" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="G43" s="4">
         <v>20.5</v>
@@ -2460,15 +2455,15 @@
       <c r="B44" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C44" s="9">
-        <v>2</v>
+      <c r="C44" s="9" t="s">
+        <v>129</v>
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="8">
         <v>7</v>
       </c>
-      <c r="F44" s="4">
-        <v>1</v>
+      <c r="F44" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="G44" s="4">
         <v>20.5</v>
@@ -2495,15 +2490,15 @@
       <c r="B45" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C45" s="9">
-        <v>2</v>
+      <c r="C45" s="9" t="s">
+        <v>129</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="8">
         <v>8</v>
       </c>
-      <c r="F45" s="4">
-        <v>1</v>
+      <c r="F45" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="G45" s="4">
         <v>20.5</v>
@@ -2530,15 +2525,15 @@
       <c r="B46" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C46" s="9">
-        <v>2</v>
+      <c r="C46" s="9" t="s">
+        <v>129</v>
       </c>
       <c r="D46" s="4"/>
       <c r="E46" s="21">
         <v>9</v>
       </c>
-      <c r="F46" s="22">
-        <v>2</v>
+      <c r="F46" s="22" t="s">
+        <v>131</v>
       </c>
       <c r="G46" s="22">
         <v>0</v>
@@ -2565,15 +2560,15 @@
       <c r="B47" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C47" s="9">
-        <v>2</v>
+      <c r="C47" s="9" t="s">
+        <v>129</v>
       </c>
       <c r="D47" s="4"/>
       <c r="E47" s="32">
         <v>10</v>
       </c>
-      <c r="F47" s="6">
-        <v>1</v>
+      <c r="F47" s="6" t="s">
+        <v>130</v>
       </c>
       <c r="G47" s="6">
         <v>29</v>
@@ -2600,15 +2595,15 @@
       <c r="B48" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C48" s="9">
-        <v>2</v>
+      <c r="C48" s="9" t="s">
+        <v>129</v>
       </c>
       <c r="D48" s="4"/>
       <c r="E48" s="8">
         <v>11</v>
       </c>
-      <c r="F48" s="4">
-        <v>2</v>
+      <c r="F48" s="4" t="s">
+        <v>131</v>
       </c>
       <c r="G48" s="4">
         <v>0</v>
@@ -2635,15 +2630,15 @@
       <c r="B49" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C49" s="9">
-        <v>2</v>
+      <c r="C49" s="9" t="s">
+        <v>129</v>
       </c>
       <c r="D49" s="4"/>
       <c r="E49" s="8">
         <v>12</v>
       </c>
-      <c r="F49" s="4">
-        <v>3</v>
+      <c r="F49" s="4" t="s">
+        <v>132</v>
       </c>
       <c r="G49" s="4">
         <v>0</v>
@@ -2670,15 +2665,15 @@
       <c r="B50" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C50" s="9">
-        <v>2</v>
+      <c r="C50" s="9" t="s">
+        <v>129</v>
       </c>
       <c r="D50" s="4"/>
       <c r="E50" s="8">
         <v>13</v>
       </c>
-      <c r="F50" s="4">
-        <v>2</v>
+      <c r="F50" s="4" t="s">
+        <v>131</v>
       </c>
       <c r="G50" s="4">
         <v>0</v>
@@ -2705,15 +2700,15 @@
       <c r="B51" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="C51" s="9">
-        <v>2</v>
+      <c r="C51" s="9" t="s">
+        <v>129</v>
       </c>
       <c r="D51" s="4"/>
       <c r="E51" s="8">
         <v>14</v>
       </c>
-      <c r="F51" s="4">
-        <v>3</v>
+      <c r="F51" s="4" t="s">
+        <v>132</v>
       </c>
       <c r="G51" s="4">
         <v>0</v>
@@ -2740,15 +2735,15 @@
       <c r="B52" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="C52" s="24">
-        <v>2</v>
+      <c r="C52" s="24" t="s">
+        <v>129</v>
       </c>
       <c r="D52" s="4"/>
       <c r="E52" s="8">
         <v>15</v>
       </c>
-      <c r="F52" s="4">
-        <v>1</v>
+      <c r="F52" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="G52" s="4">
         <v>29</v>
@@ -2776,8 +2771,8 @@
       <c r="E53" s="21">
         <v>16</v>
       </c>
-      <c r="F53" s="22">
-        <v>1</v>
+      <c r="F53" s="22" t="s">
+        <v>130</v>
       </c>
       <c r="G53" s="22">
         <v>29</v>
@@ -2805,8 +2800,8 @@
       <c r="E54" s="8">
         <v>17</v>
       </c>
-      <c r="F54" s="4">
-        <v>1</v>
+      <c r="F54" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="G54" s="4">
         <v>22</v>
@@ -2834,8 +2829,8 @@
       <c r="E55" s="8">
         <v>18</v>
       </c>
-      <c r="F55" s="4">
-        <v>1</v>
+      <c r="F55" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="G55" s="4">
         <v>22</v>
@@ -2863,8 +2858,8 @@
       <c r="E56" s="8">
         <v>19</v>
       </c>
-      <c r="F56" s="4">
-        <v>2</v>
+      <c r="F56" s="4" t="s">
+        <v>131</v>
       </c>
       <c r="G56" s="4">
         <v>0</v>
@@ -2888,14 +2883,13 @@
       <c r="A57" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B57" s="6"/>
-      <c r="C57" s="7"/>
+      <c r="B57" s="7"/>
       <c r="D57" s="4"/>
       <c r="E57" s="8">
         <v>20</v>
       </c>
-      <c r="F57" s="4">
-        <v>1</v>
+      <c r="F57" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="G57" s="4">
         <v>22</v>
@@ -2917,14 +2911,13 @@
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" s="8"/>
-      <c r="B58" s="4"/>
-      <c r="C58" s="9"/>
+      <c r="B58" s="9"/>
       <c r="D58" s="4"/>
       <c r="E58" s="8">
         <v>21</v>
       </c>
-      <c r="F58" s="4">
-        <v>2</v>
+      <c r="F58" s="4" t="s">
+        <v>131</v>
       </c>
       <c r="G58" s="4">
         <v>0</v>
@@ -2948,18 +2941,15 @@
       <c r="A59" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B59" s="11" t="s">
+      <c r="B59" s="14" t="s">
         <v>26</v>
-      </c>
-      <c r="C59" s="17" t="s">
-        <v>27</v>
       </c>
       <c r="D59" s="4"/>
       <c r="E59" s="21">
         <v>22</v>
       </c>
-      <c r="F59" s="22">
-        <v>3</v>
+      <c r="F59" s="22" t="s">
+        <v>132</v>
       </c>
       <c r="G59" s="22">
         <v>0</v>
@@ -2983,18 +2973,15 @@
       <c r="A60" s="8">
         <v>1</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B60" s="9" t="s">
         <v>56</v>
-      </c>
-      <c r="C60" s="9">
-        <v>3</v>
       </c>
       <c r="D60" s="4"/>
       <c r="E60" s="8">
         <v>23</v>
       </c>
-      <c r="F60" s="4">
-        <v>2</v>
+      <c r="F60" s="4" t="s">
+        <v>131</v>
       </c>
       <c r="G60" s="4">
         <v>0</v>
@@ -3018,18 +3005,15 @@
       <c r="A61" s="8">
         <v>2</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" s="9" t="s">
         <v>60</v>
-      </c>
-      <c r="C61" s="9">
-        <v>3</v>
       </c>
       <c r="D61" s="4"/>
       <c r="E61" s="8">
         <v>24</v>
       </c>
-      <c r="F61" s="4">
-        <v>1</v>
+      <c r="F61" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="G61" s="4">
         <v>98</v>
@@ -3053,18 +3037,15 @@
       <c r="A62" s="8">
         <v>3</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="9" t="s">
         <v>93</v>
-      </c>
-      <c r="C62" s="9">
-        <v>1</v>
       </c>
       <c r="D62" s="4"/>
       <c r="E62" s="8">
         <v>25</v>
       </c>
-      <c r="F62" s="4">
-        <v>2</v>
+      <c r="F62" s="4" t="s">
+        <v>131</v>
       </c>
       <c r="G62" s="4">
         <v>0</v>
@@ -3088,18 +3069,15 @@
       <c r="A63" s="8">
         <v>4</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="9" t="s">
         <v>69</v>
-      </c>
-      <c r="C63" s="9">
-        <v>7</v>
       </c>
       <c r="D63" s="4"/>
       <c r="E63" s="8">
         <v>26</v>
       </c>
-      <c r="F63" s="4">
-        <v>3</v>
+      <c r="F63" s="4" t="s">
+        <v>132</v>
       </c>
       <c r="G63" s="4">
         <v>0</v>
@@ -3123,18 +3101,15 @@
       <c r="A64" s="8">
         <v>5</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B64" s="9" t="s">
         <v>85</v>
-      </c>
-      <c r="C64" s="9">
-        <v>3</v>
       </c>
       <c r="D64" s="4"/>
       <c r="E64" s="8">
         <v>27</v>
       </c>
-      <c r="F64" s="4">
-        <v>2</v>
+      <c r="F64" s="4" t="s">
+        <v>131</v>
       </c>
       <c r="G64" s="4">
         <v>0</v>
@@ -3158,18 +3133,15 @@
       <c r="A65" s="8">
         <v>6</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B65" s="9" t="s">
         <v>92</v>
-      </c>
-      <c r="C65" s="9">
-        <v>4</v>
       </c>
       <c r="D65" s="4"/>
       <c r="E65" s="21">
         <v>28</v>
       </c>
-      <c r="F65" s="22">
-        <v>3</v>
+      <c r="F65" s="22" t="s">
+        <v>132</v>
       </c>
       <c r="G65" s="22">
         <v>0</v>
@@ -3193,11 +3165,8 @@
       <c r="A66" s="8">
         <v>7</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B66" s="9" t="s">
         <v>94</v>
-      </c>
-      <c r="C66" s="9">
-        <v>1</v>
       </c>
       <c r="D66" s="4"/>
       <c r="E66" s="4"/>
@@ -3218,11 +3187,8 @@
       <c r="A67" s="8">
         <v>8</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B67" s="9" t="s">
         <v>95</v>
-      </c>
-      <c r="C67" s="9">
-        <v>10</v>
       </c>
       <c r="D67" s="4"/>
       <c r="E67" s="4"/>
@@ -3243,11 +3209,8 @@
       <c r="A68" s="8">
         <v>9</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B68" s="9" t="s">
         <v>96</v>
-      </c>
-      <c r="C68" s="9">
-        <v>8</v>
       </c>
       <c r="D68" s="4"/>
       <c r="E68" s="4"/>
@@ -3268,11 +3231,8 @@
       <c r="A69" s="8">
         <v>10</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B69" s="9" t="s">
         <v>97</v>
-      </c>
-      <c r="C69" s="9">
-        <v>6</v>
       </c>
       <c r="D69" s="4"/>
       <c r="E69" s="4"/>
@@ -3293,11 +3253,8 @@
       <c r="A70" s="21">
         <v>11</v>
       </c>
-      <c r="B70" s="22" t="s">
+      <c r="B70" s="24" t="s">
         <v>98</v>
-      </c>
-      <c r="C70" s="24">
-        <v>2</v>
       </c>
       <c r="D70" s="4"/>
       <c r="E70" s="4"/>
@@ -3846,8 +3803,8 @@
       <c r="B90" s="9"/>
       <c r="C90" s="4"/>
       <c r="D90" s="8"/>
-      <c r="E90" s="45"/>
-      <c r="F90" s="45"/>
+      <c r="E90" s="4"/>
+      <c r="F90" s="4"/>
       <c r="G90" s="9"/>
       <c r="H90" s="4"/>
       <c r="I90" s="4"/>
@@ -3871,11 +3828,11 @@
       <c r="D91" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="E91" s="46" t="s">
+      <c r="E91" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="F91" s="46" t="s">
-        <v>128</v>
+      <c r="F91" s="11" t="s">
+        <v>124</v>
       </c>
       <c r="G91" s="14" t="s">
         <v>42</v>
@@ -3902,10 +3859,10 @@
       <c r="D92" s="8">
         <v>1</v>
       </c>
-      <c r="E92" s="45" t="s">
+      <c r="E92" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="F92" s="45" t="s">
+      <c r="F92" s="4" t="s">
         <v>118</v>
       </c>
       <c r="G92" s="38">
@@ -3933,10 +3890,10 @@
       <c r="D93" s="8">
         <v>2</v>
       </c>
-      <c r="E93" s="45" t="s">
+      <c r="E93" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="F93" s="45" t="s">
+      <c r="F93" s="4" t="s">
         <v>118</v>
       </c>
       <c r="G93" s="38">
@@ -3964,10 +3921,10 @@
       <c r="D94" s="8">
         <v>3</v>
       </c>
-      <c r="E94" s="45" t="s">
+      <c r="E94" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="F94" s="45" t="s">
+      <c r="F94" s="4" t="s">
         <v>118</v>
       </c>
       <c r="G94" s="38">
@@ -3995,10 +3952,10 @@
       <c r="D95" s="8">
         <v>4</v>
       </c>
-      <c r="E95" s="45" t="s">
+      <c r="E95" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="F95" s="45" t="s">
+      <c r="F95" s="4" t="s">
         <v>119</v>
       </c>
       <c r="G95" s="38">
@@ -4026,10 +3983,10 @@
       <c r="D96" s="8">
         <v>5</v>
       </c>
-      <c r="E96" s="45" t="s">
+      <c r="E96" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="F96" s="45" t="s">
+      <c r="F96" s="4" t="s">
         <v>120</v>
       </c>
       <c r="G96" s="38">
@@ -4057,10 +4014,10 @@
       <c r="D97" s="8">
         <v>6</v>
       </c>
-      <c r="E97" s="45" t="s">
+      <c r="E97" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="F97" s="45" t="s">
+      <c r="F97" s="4" t="s">
         <v>121</v>
       </c>
       <c r="G97" s="38">
@@ -4088,10 +4045,10 @@
       <c r="D98" s="8">
         <v>7</v>
       </c>
-      <c r="E98" s="45" t="s">
+      <c r="E98" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="F98" s="45" t="s">
+      <c r="F98" s="4" t="s">
         <v>122</v>
       </c>
       <c r="G98" s="38">
@@ -4184,8 +4141,10 @@
       <c r="D102" s="4"/>
       <c r="E102" s="4"/>
       <c r="F102" s="4"/>
-      <c r="G102" s="4"/>
-      <c r="H102" s="4"/>
+      <c r="G102" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="H102" s="7"/>
       <c r="I102" s="4"/>
       <c r="J102" s="4"/>
       <c r="K102" s="4"/>
@@ -4200,11 +4159,13 @@
       <c r="A103" s="4"/>
       <c r="B103" s="4"/>
       <c r="C103" s="4"/>
-      <c r="D103" s="4"/>
+      <c r="D103" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="E103" s="4"/>
       <c r="F103" s="4"/>
-      <c r="G103" s="4"/>
-      <c r="H103" s="4"/>
+      <c r="G103" s="8"/>
+      <c r="H103" s="9"/>
       <c r="I103" s="4"/>
       <c r="J103" s="4"/>
       <c r="K103" s="4"/>
@@ -4219,11 +4180,17 @@
       <c r="A104" s="4"/>
       <c r="B104" s="4"/>
       <c r="C104" s="4"/>
-      <c r="D104" s="4"/>
+      <c r="D104" s="2" t="s">
+        <v>87</v>
+      </c>
       <c r="E104" s="4"/>
       <c r="F104" s="4"/>
-      <c r="G104" s="4"/>
-      <c r="H104" s="4"/>
+      <c r="G104" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="H104" s="17" t="s">
+        <v>27</v>
+      </c>
       <c r="I104" s="4"/>
       <c r="J104" s="4"/>
       <c r="K104" s="4"/>
@@ -4238,11 +4205,17 @@
       <c r="A105" s="4"/>
       <c r="B105" s="4"/>
       <c r="C105" s="4"/>
-      <c r="D105" s="4"/>
+      <c r="D105" s="3" t="s">
+        <v>86</v>
+      </c>
       <c r="E105" s="4"/>
       <c r="F105" s="4"/>
-      <c r="G105" s="4"/>
-      <c r="H105" s="4"/>
+      <c r="G105" s="45">
+        <v>1</v>
+      </c>
+      <c r="H105" s="46">
+        <v>3</v>
+      </c>
       <c r="I105" s="4"/>
       <c r="J105" s="4"/>
       <c r="K105" s="4"/>
@@ -4260,8 +4233,12 @@
       <c r="D106" s="4"/>
       <c r="E106" s="4"/>
       <c r="F106" s="4"/>
-      <c r="G106" s="4"/>
-      <c r="H106" s="4"/>
+      <c r="G106" s="45">
+        <v>1</v>
+      </c>
+      <c r="H106" s="46">
+        <v>3</v>
+      </c>
       <c r="I106" s="4"/>
       <c r="J106" s="4"/>
       <c r="K106" s="4"/>
@@ -4279,8 +4256,12 @@
       <c r="D107" s="4"/>
       <c r="E107" s="4"/>
       <c r="F107" s="4"/>
-      <c r="G107" s="4"/>
-      <c r="H107" s="4"/>
+      <c r="G107" s="45">
+        <v>1</v>
+      </c>
+      <c r="H107" s="46">
+        <v>3</v>
+      </c>
       <c r="I107" s="4"/>
       <c r="J107" s="4"/>
       <c r="K107" s="4"/>
@@ -4298,8 +4279,12 @@
       <c r="D108" s="4"/>
       <c r="E108" s="4"/>
       <c r="F108" s="4"/>
-      <c r="G108" s="4"/>
-      <c r="H108" s="4"/>
+      <c r="G108" s="45">
+        <v>4</v>
+      </c>
+      <c r="H108" s="46">
+        <v>7</v>
+      </c>
       <c r="I108" s="4"/>
       <c r="J108" s="4"/>
       <c r="K108" s="4"/>
@@ -4317,8 +4302,12 @@
       <c r="D109" s="4"/>
       <c r="E109" s="4"/>
       <c r="F109" s="4"/>
-      <c r="G109" s="4"/>
-      <c r="H109" s="4"/>
+      <c r="G109" s="45">
+        <v>5</v>
+      </c>
+      <c r="H109" s="46">
+        <v>3</v>
+      </c>
       <c r="I109" s="4"/>
       <c r="J109" s="4"/>
       <c r="K109" s="4"/>
@@ -4336,8 +4325,12 @@
       <c r="D110" s="4"/>
       <c r="E110" s="4"/>
       <c r="F110" s="4"/>
-      <c r="G110" s="4"/>
-      <c r="H110" s="4"/>
+      <c r="G110" s="45">
+        <v>6</v>
+      </c>
+      <c r="H110" s="46">
+        <v>4</v>
+      </c>
       <c r="I110" s="4"/>
       <c r="J110" s="4"/>
       <c r="K110" s="4"/>
@@ -4355,8 +4348,12 @@
       <c r="D111" s="4"/>
       <c r="E111" s="4"/>
       <c r="F111" s="4"/>
-      <c r="G111" s="4"/>
-      <c r="H111" s="4"/>
+      <c r="G111" s="45">
+        <v>7</v>
+      </c>
+      <c r="H111" s="46">
+        <v>1</v>
+      </c>
       <c r="I111" s="4"/>
       <c r="J111" s="4"/>
       <c r="K111" s="4"/>
@@ -4374,8 +4371,12 @@
       <c r="D112" s="4"/>
       <c r="E112" s="4"/>
       <c r="F112" s="4"/>
-      <c r="G112" s="4"/>
-      <c r="H112" s="4"/>
+      <c r="G112" s="45">
+        <v>8</v>
+      </c>
+      <c r="H112" s="46">
+        <v>10</v>
+      </c>
       <c r="I112" s="4"/>
       <c r="J112" s="4"/>
       <c r="K112" s="4"/>
@@ -4393,8 +4394,12 @@
       <c r="D113" s="4"/>
       <c r="E113" s="4"/>
       <c r="F113" s="4"/>
-      <c r="G113" s="4"/>
-      <c r="H113" s="4"/>
+      <c r="G113" s="45">
+        <v>9</v>
+      </c>
+      <c r="H113" s="46">
+        <v>8</v>
+      </c>
       <c r="I113" s="4"/>
       <c r="J113" s="4"/>
       <c r="K113" s="4"/>
@@ -4412,8 +4417,12 @@
       <c r="D114" s="4"/>
       <c r="E114" s="4"/>
       <c r="F114" s="4"/>
-      <c r="G114" s="4"/>
-      <c r="H114" s="4"/>
+      <c r="G114" s="8">
+        <v>10</v>
+      </c>
+      <c r="H114" s="9">
+        <v>6</v>
+      </c>
       <c r="I114" s="4"/>
       <c r="J114" s="4"/>
       <c r="K114" s="4"/>
@@ -4431,8 +4440,12 @@
       <c r="D115" s="4"/>
       <c r="E115" s="4"/>
       <c r="F115" s="4"/>
-      <c r="G115" s="4"/>
-      <c r="H115" s="4"/>
+      <c r="G115" s="21">
+        <v>11</v>
+      </c>
+      <c r="H115" s="24">
+        <v>2</v>
+      </c>
       <c r="I115" s="4"/>
       <c r="J115" s="4"/>
       <c r="K115" s="4"/>
@@ -4963,15 +4976,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100B2C7AFC8D3671240B5A22E09B307AEF3" ma:contentTypeVersion="15" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="18f5372394ed4318cdbf062904967825">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="bfd064f1-60da-4f0f-a847-89d2c1a6c329" xmlns:ns4="44e2c5d4-dcdf-4cd8-88c2-2d4d1c90d35d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="284b2db933a0d2bc0e19e591f6d49d7f" ns3:_="" ns4:_="">
     <xsd:import namespace="bfd064f1-60da-4f0f-a847-89d2c1a6c329"/>
@@ -5204,6 +5208,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -5213,14 +5226,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{625651FB-5DE0-467D-880A-FE0D31657576}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42502E2E-4434-47F6-BDEB-BB942FCD563D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5239,19 +5244,27 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{625651FB-5DE0-467D-880A-FE0D31657576}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B93F357-B08C-46F6-8993-B6096D7632F5}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="bfd064f1-60da-4f0f-a847-89d2c1a6c329"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="44e2c5d4-dcdf-4cd8-88c2-2d4d1c90d35d"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="44e2c5d4-dcdf-4cd8-88c2-2d4d1c90d35d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>